<commit_message>
Updated income and bills import functionality
</commit_message>
<xml_diff>
--- a/Export Files/My Bills and Income.xlsx
+++ b/Export Files/My Bills and Income.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>ID</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>Expense Description</t>
-  </si>
-  <si>
-    <t>User ID</t>
   </si>
   <si>
     <t>Income Category</t>
@@ -84,7 +81,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -95,7 +92,6 @@
     <col min="3" max="3" width="16.9375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="8.42578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="19.14453125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="7.57421875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -114,9 +110,6 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -125,7 +118,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -136,7 +129,6 @@
     <col min="3" max="3" width="16.203125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="7.6875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="18.41015625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="7.57421875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -147,16 +139,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>